<commit_message>
* Inventory, Reward 구현.
</commit_message>
<xml_diff>
--- a/input/Domains/Game/PurchaseTable.xlsx
+++ b/input/Domains/Game/PurchaseTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maoshy/Documents/Projects/devian/input/Domains/Purchase/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maoshy/Documents/Projects/devian/input/Domains/Game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE2000D-B450-8648-B9E5-2E603582B7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D0CEAC-2053-3248-966E-7417FAA43672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="500" windowWidth="37020" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>internalProductId</t>
   </si>
   <si>
+    <t>rewardId</t>
+  </si>
+  <si>
     <t>kind</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>내부 상품 ID (정본)</t>
   </si>
   <si>
+    <t>Reward Key (REWARD.rewardId(pk))</t>
+  </si>
+  <si>
     <t>상품 타입 (Consumable/Rental/Subscription/SeasonPass)</t>
   </si>
   <si>
@@ -67,20 +73,16 @@
     <t>Google Play SKU</t>
   </si>
   <si>
+    <t>com.devian.framework.noads_month</t>
+  </si>
+  <si>
     <t>Rental</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.devian.framework.noads_subscription</t>
   </si>
   <si>
     <t>Subscription</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.devian.framework.noads_month</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.devian.framework.noads_subscription</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -427,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,10 +440,10 @@
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="40.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,69 +462,78 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
         <v>12</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>